<commit_message>
Adjust color axis values
</commit_message>
<xml_diff>
--- a/3-climate-change/data/CO2_emissions_2012.xlsx
+++ b/3-climate-change/data/CO2_emissions_2012.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28720" yWindow="-3600" windowWidth="38400" windowHeight="21140" activeTab="2"/>
+    <workbookView xWindow="28720" yWindow="-3600" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ok" sheetId="4" r:id="rId2"/>
-    <sheet name="ok (2)" sheetId="6" r:id="rId3"/>
+    <sheet name="CURATED" sheetId="6" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CURATED!$A$1:$C$70</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="98">
   <si>
     <t>US</t>
   </si>
@@ -313,6 +316,9 @@
   <si>
     <t>COUNTRY</t>
   </si>
+  <si>
+    <t>string1</t>
+  </si>
 </sst>
 </file>
 
@@ -376,10 +382,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,16 +421,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="33">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -705,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC96"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="X1" sqref="A1:X1048576"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10373,7 +10423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -10381,567 +10433,851 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1">
+        <v>2625729.932736964</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("['",A2,"', ",INT(B2),"],")</f>
+        <v>['China', 2625729],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
         <v>1396790.7648451091</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="0">CONCATENATE("['",A3,"', ",INT(B3),"],")</f>
+        <v>['US', 1396790],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1">
+        <v>611226.32316958916</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>['India', 611226],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1">
+        <v>491840.33543909399</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>['Russian Federation', 491840],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1">
+        <v>342270.02191037923</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>['Japan', 342270],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1">
+        <v>330941.99557889096</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>['Total Africa', 330941],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>199716.14896148487</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>['Germany', 199716],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1">
+        <v>166679.15746470925</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>['South Korea', 166679],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1">
+        <v>164497.67410158212</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>['Iran', 164497],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1">
+        <v>137877.70810957171</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>['Saudi Arabia', 137877],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B12" s="1">
         <v>137819.83011260908</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>['Canada', 137819],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1">
+        <v>129987.63422779723</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>['Indonesia', 129987],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B14" s="1">
         <v>129942.37582630581</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>53547.937624577215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>['Mexico', 129942],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1">
+        <v>128494.04064963351</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>['United Kingdom', 128494],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1">
+        <v>125741.87230816028</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>['South Africa', 125741],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B17" s="1">
         <v>122082.41549725691</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>24778.588030401319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>21981.374513227292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>9513.9366238645707</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>17805.006345243961</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>12835.629274219658</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>56599.572881389635</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>16312.18374570173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13897.073742635057</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>16907.219335105743</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="1">
-        <v>27050.534949886813</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1">
-        <v>12414.359814007172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>['Brazil', 122082],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1">
-        <v>28288.208953162346</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>108880.73748252774</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>['Other Africa', 108880],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
-        <v>10007.632989994278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>102368.62639672708</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>['Italy', 102368],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1">
-        <v>13055.362836911692</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>101147.00533811742</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>['Australia', 101147],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>93712.565440615203</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>['France', 93712],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1">
-        <v>199716.14896148487</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>88383.891280419644</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>['Ukraine', 88383],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="1">
+        <v>88044.0968255185</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>['Thailand', 88044],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1">
+        <v>84860.632914475194</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>['Turkey', 84860],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1">
+        <v>83894.730079754285</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>['Poland', 83894],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1">
+        <v>79616.824283165581</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>['Kazakhstan', 79616],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1">
+        <v>75676.701894265265</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>['Spain', 75676],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1">
+        <v>71558.817520396173</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>['Taiwan', 71558],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="1">
+        <v>58952.860837533932</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>['Malaysia', 58952],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1">
+        <v>58649.554507574256</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>['Egypt', 58649],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1">
+        <v>56599.572881389635</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>['Venezuela', 56599],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1">
+        <v>53547.937624577215</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>['Argentina', 53547],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="1">
+        <v>46720.745295175308</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>['United Arab Emirates', 46720],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45421.391169338378</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>['Netherlands', 45421],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44624.503473974044</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>['Vietnam', 44624],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44051.877142625519</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>['Pakistan', 44051],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="1">
+        <v>37669.831280628729</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>['Algeria', 37669],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1">
+        <v>30047.57970204344</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>['Uzbekistan', 30047],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1">
+        <v>28288.208953162346</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>['Czech Republic', 28288],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="1">
+        <v>27050.534949886813</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>['Belgium', 27050],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="1">
+        <v>26357.955150148671</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>['Kuwait', 26357],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="1">
+        <v>24778.588030401319</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>['Chile', 24778],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="1">
+        <v>24662.641373500301</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>['Qatar', 24662],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="1">
+        <v>23624.612841412923</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>['Philippines', 23624],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B45" s="1">
         <v>22289.532632336344</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greece', 22289],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="1">
+        <v>22210.831051712248</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>['Romania', 22210],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1">
+        <v>21981.374513227292</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>['Colombia', 21981],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20928.274947645612</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>['Israel', 20928],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="1">
+        <v>17805.006345243961</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>['Peru', 17805],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="1">
+        <v>17707.259472079972</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>['Bangladesh', 17707],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="1">
+        <v>16907.219335105743</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>['Belarus', 16907],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="1">
+        <v>16312.18374570173</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>['Austria', 16312],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="1">
+        <v>15835.25608083871</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>['Norway', 15835],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="1">
+        <v>15059.267237126263</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>['Turkmenistan', 15059],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="1">
+        <v>14367.716966656817</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>['Portugal', 14367],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="1">
+        <v>13897.073742635057</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>['Azerbaijan', 13897],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="1">
+        <v>13055.362836911692</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>['Finland', 13055],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="1">
+        <v>12835.629274219658</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>['Trinidad &amp; Tobago', 12835],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B59" s="1">
         <v>12675.221851083235</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>['Hungary', 12675],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="1">
+        <v>12414.359814007172</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>['Bulgaria', 12414],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" s="1">
+        <v>12232.977073612488</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>['Sweden', 12232],</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="1">
+        <v>10483.038448486963</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>['China Hong Kong SAR', 10483],</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="1">
+        <v>10366.176395978035</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>['Switzerland', 10366],</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="1">
+        <v>10007.632989994278</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>['Denmark', 10007],</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B65" s="1">
         <v>9889.6927845552054</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="1">
-        <v>102368.62639672708</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>79616.824283165581</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>['Republic of Ireland', 9889],</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="1">
+        <v>9689.3621084826627</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>['Slovakia', 9689],</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="1">
+        <v>9513.9366238645707</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C70" si="1">CONCATENATE("['",A67,"', ",INT(B67),"],")</f>
+        <v>['Ecuador', 9513],</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>8852.4563185252373</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>['New Zealand', 8852],</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B69" s="1">
         <v>3718.3905708440489</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1">
-        <v>45421.391169338378</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <v>15835.25608083871</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="1">
-        <v>83894.730079754285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1">
-        <v>14367.716966656817</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1">
-        <v>22210.831051712248</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1">
-        <v>491840.33543909399</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1">
-        <v>9689.3621084826627</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="1">
-        <v>75676.701894265265</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="1">
-        <v>12232.977073612488</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="1">
-        <v>10366.176395978035</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="1">
-        <v>84860.632914475194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="1">
-        <v>15059.267237126263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="1">
-        <v>88383.891280419644</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1">
-        <v>128494.04064963351</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="1">
-        <v>30047.57970204344</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="1">
-        <v>164497.67410158212</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="1">
-        <v>20928.274947645612</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="1">
-        <v>26357.955150148671</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="1">
-        <v>24662.641373500301</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="1">
-        <v>137877.70810957171</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="1">
-        <v>46720.745295175308</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="1">
-        <v>37669.831280628729</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="1">
-        <v>58649.554507574256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="1">
-        <v>125741.87230816028</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="1">
-        <v>108880.73748252774</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="1">
-        <v>330941.99557889096</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="1">
-        <v>101147.00533811742</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="1">
-        <v>17707.259472079972</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="1">
-        <v>2625729.932736964</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="1">
-        <v>10483.038448486963</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59" s="1">
-        <v>611226.32316958916</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" s="1">
-        <v>129987.63422779723</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" s="1">
-        <v>342270.02191037923</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="1">
-        <v>58952.860837533932</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="1">
-        <v>8852.4563185252373</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="1">
-        <v>44051.877142625519</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="1">
-        <v>23624.612841412923</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>['Lithuania', 3718],</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B70" s="1">
         <v>3587.6411665787928</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="1">
-        <v>166679.15746470925</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68" s="1">
-        <v>71558.817520396173</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B69" s="1">
-        <v>88044.0968255185</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70" s="1">
-        <v>44624.503473974044</v>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>['Singapore', 3587],</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C70">
+    <sortState ref="A2:C70">
+      <sortCondition descending="1" ref="B1:B70"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added CO2 per capita
</commit_message>
<xml_diff>
--- a/3-climate-change/data/CO2_emissions_2012.xlsx
+++ b/3-climate-change/data/CO2_emissions_2012.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28720" yWindow="-3600" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="28720" yWindow="-3600" windowWidth="38400" windowHeight="21140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ok" sheetId="4" r:id="rId2"/>
     <sheet name="CURATED" sheetId="6" r:id="rId3"/>
+    <sheet name="popn" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CURATED!$A$1:$C$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CURATED!$A$1:$C$69</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="285">
   <si>
     <t>US</t>
   </si>
@@ -318,6 +319,567 @@
   </si>
   <si>
     <t>string1</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population2012</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Arab World</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bahamas, The</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Central Europe and the Baltics</t>
+  </si>
+  <si>
+    <t>Channel Islands</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Congo, Rep.</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Caribbean small states</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>East Asia &amp; Pacific (developing only)</t>
+  </si>
+  <si>
+    <t>East Asia &amp; Pacific (all income levels)</t>
+  </si>
+  <si>
+    <t>Europe &amp; Central Asia (developing only)</t>
+  </si>
+  <si>
+    <t>Europe &amp; Central Asia (all income levels)</t>
+  </si>
+  <si>
+    <t>Euro area</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t>Fragile and conflict affected situations</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Faeroe Islands</t>
+  </si>
+  <si>
+    <t>Micronesia, Fed. Sts.</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Gambia, The</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>High income</t>
+  </si>
+  <si>
+    <t>Hong Kong SAR, China</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Heavily indebted poor countries (HIPC)</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kyrgyz Republic</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>St. Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Latin America &amp; Caribbean (developing only)</t>
+  </si>
+  <si>
+    <t>Lao PDR</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>St. Lucia</t>
+  </si>
+  <si>
+    <t>Latin America &amp; Caribbean (all income levels)</t>
+  </si>
+  <si>
+    <t>Least developed countries: UN classification</t>
+  </si>
+  <si>
+    <t>Low income</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Lower middle income</t>
+  </si>
+  <si>
+    <t>Low &amp; middle income</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Macao SAR, China</t>
+  </si>
+  <si>
+    <t>St. Martin (French part)</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Middle East &amp; North Africa (all income levels)</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Middle income</t>
+  </si>
+  <si>
+    <t>Macedonia, FYR</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Middle East &amp; North Africa (developing only)</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>High income: nonOECD</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>High income: OECD</t>
+  </si>
+  <si>
+    <t>OECD members</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Other small states</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Pacific island small states</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>South Asia</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Sub-Saharan Africa (developing only)</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Sub-Saharan Africa (all income levels)</t>
+  </si>
+  <si>
+    <t>Small states</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Slovak Republic</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Sint Maarten (Dutch part)</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Upper middle income</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>St. Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Virgin Islands (U.S.)</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>West Bank and Gaza</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>Yemen, Rep.</t>
+  </si>
+  <si>
+    <t>Congo, Dem. Rep.</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>POPULATION</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>PERCAPITACO2</t>
   </si>
 </sst>
 </file>
@@ -382,7 +944,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,12 +978,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="39">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -438,6 +1007,9 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -453,6 +1025,9 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -755,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -10421,19 +10996,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C70"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -10443,8 +11021,14 @@
       <c r="C1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -10455,8 +11039,20 @@
         <f>CONCATENATE("['",A2,"', ",INT(B2),"],")</f>
         <v>['China', 2625729],</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <f>VLOOKUP(A2,popn!$A$2:$B$248,2,0)</f>
+        <v>1350695000</v>
+      </c>
+      <c r="E2" s="2">
+        <f>B2/D2*1000</f>
+        <v>1.9439843434209529</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE("['",A2,"', ",E2,"],")</f>
+        <v>['China', 1.94398434342095],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -10464,11 +11060,23 @@
         <v>1396790.7648451091</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C66" si="0">CONCATENATE("['",A3,"', ",INT(B3),"],")</f>
+        <f t="shared" ref="C3:C65" si="0">CONCATENATE("['",A3,"', ",INT(B3),"],")</f>
         <v>['US', 1396790],</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <f>VLOOKUP(A3,popn!$A$2:$B$248,2,0)</f>
+        <v>313873685</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E66" si="1">B3/D3*1000</f>
+        <v>4.4501684327091935</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="2">CONCATENATE("['",A3,"', ",E3,"],")</f>
+        <v>['US', 4.45016843270919],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -10479,8 +11087,20 @@
         <f t="shared" si="0"/>
         <v>['India', 611226],</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <f>VLOOKUP(A4,popn!$A$2:$B$248,2,0)</f>
+        <v>1236686732</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49424507221897584</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>['India', 0.494245072218976],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -10491,8 +11111,20 @@
         <f t="shared" si="0"/>
         <v>['Russian Federation', 491840],</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <f>VLOOKUP(A5,popn!$A$2:$B$248,2,0)</f>
+        <v>143178000</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4351669630745922</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>['Russian Federation', 3.43516696307459],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -10503,777 +11135,1517 @@
         <f t="shared" si="0"/>
         <v>['Japan', 342270],</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <f>VLOOKUP(A6,popn!$A$2:$B$248,2,0)</f>
+        <v>127561489</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6831767533724791</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>['Japan', 2.68317675337248],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
-        <v>330941.99557889096</v>
+        <v>199716.14896148487</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>['Total Africa', 330941],</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>['Germany', 199716],</v>
+      </c>
+      <c r="D7">
+        <f>VLOOKUP(A7,popn!$A$2:$B$248,2,0)</f>
+        <v>80425823</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4832341344083586</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>['Germany', 2.48323413440836],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1">
-        <v>199716.14896148487</v>
+        <v>166679.15746470925</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>['Germany', 199716],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>['South Korea', 166679],</v>
+      </c>
+      <c r="D8">
+        <f>VLOOKUP(A8,popn!$A$2:$B$248,2,0)</f>
+        <v>50004441</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3332870867351412</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>['South Korea', 3.33328708673514],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
-        <v>166679.15746470925</v>
+        <v>164497.67410158212</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>['South Korea', 166679],</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>['Iran', 164497],</v>
+      </c>
+      <c r="D9">
+        <f>VLOOKUP(A9,popn!$A$2:$B$248,2,0)</f>
+        <v>76424443</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1524222832946536</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>['Iran', 2.15242228329465],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1">
-        <v>164497.67410158212</v>
+        <v>137877.70810957171</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>['Iran', 164497],</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>['Saudi Arabia', 137877],</v>
+      </c>
+      <c r="D10">
+        <f>VLOOKUP(A10,popn!$A$2:$B$248,2,0)</f>
+        <v>28287855</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>4.8740955477031296</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>['Saudi Arabia', 4.87409554770313],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>137877.70810957171</v>
+        <v>137819.83011260908</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>['Saudi Arabia', 137877],</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>['Canada', 137819],</v>
+      </c>
+      <c r="D11">
+        <f>VLOOKUP(A11,popn!$A$2:$B$248,2,0)</f>
+        <v>34752128</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>3.9657954215813507</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>['Canada', 3.96579542158135],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1">
-        <v>137819.83011260908</v>
+        <v>129987.63422779723</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>['Canada', 137819],</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>['Indonesia', 129987],</v>
+      </c>
+      <c r="D12">
+        <f>VLOOKUP(A12,popn!$A$2:$B$248,2,0)</f>
+        <v>246864191</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.52655524359868466</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>['Indonesia', 0.526555243598685],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1">
-        <v>129987.63422779723</v>
+        <v>129942.37582630581</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>['Indonesia', 129987],</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>['Mexico', 129942],</v>
+      </c>
+      <c r="D13">
+        <f>VLOOKUP(A13,popn!$A$2:$B$248,2,0)</f>
+        <v>120847477</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0752593190365556</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>['Mexico', 1.07525931903656],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1">
-        <v>129942.37582630581</v>
+        <v>128494.04064963351</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>['Mexico', 129942],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>['United Kingdom', 128494],</v>
+      </c>
+      <c r="D14">
+        <f>VLOOKUP(A14,popn!$A$2:$B$248,2,0)</f>
+        <v>63700300</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0171653924649258</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>['United Kingdom', 2.01716539246493],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1">
-        <v>128494.04064963351</v>
+        <v>125741.87230816028</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>['United Kingdom', 128494],</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>['South Africa', 125741],</v>
+      </c>
+      <c r="D15">
+        <f>VLOOKUP(A15,popn!$A$2:$B$248,2,0)</f>
+        <v>52341695</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4023270990394998</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>['South Africa', 2.4023270990395],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>125741.87230816028</v>
+        <v>122082.41549725691</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>['South Africa', 125741],</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>['Brazil', 122082],</v>
+      </c>
+      <c r="D16">
+        <f>VLOOKUP(A16,popn!$A$2:$B$248,2,0)</f>
+        <v>198656019</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.614541739594897</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>['Brazil', 0.614541739594897],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1">
-        <v>122082.41549725691</v>
+        <v>108880.73748252774</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>['Brazil', 122082],</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>['Other Africa', 108880],</v>
+      </c>
+      <c r="D17" t="e">
+        <f>VLOOKUP(A17,popn!$A$2:$B$248,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
-        <v>108880.73748252774</v>
+        <v>102368.62639672708</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>['Other Africa', 108880],</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>['Italy', 102368],</v>
+      </c>
+      <c r="D18">
+        <f>VLOOKUP(A18,popn!$A$2:$B$248,2,0)</f>
+        <v>59539717</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7193334391684643</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>['Italy', 1.71933343916846],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1">
-        <v>102368.62639672708</v>
+        <v>101147.00533811742</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>['Italy', 102368],</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>['Australia', 101147],</v>
+      </c>
+      <c r="D19">
+        <f>VLOOKUP(A19,popn!$A$2:$B$248,2,0)</f>
+        <v>22728300</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4502670828050244</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>['Australia', 4.45026708280502],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>101147.00533811742</v>
+        <v>93712.565440615203</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>['Australia', 101147],</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>['France', 93712],</v>
+      </c>
+      <c r="D20">
+        <f>VLOOKUP(A20,popn!$A$2:$B$248,2,0)</f>
+        <v>65649570</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4274665537126168</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>['France', 1.42746655371262],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1">
-        <v>93712.565440615203</v>
+        <v>88383.891280419644</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>['France', 93712],</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>['Ukraine', 88383],</v>
+      </c>
+      <c r="D21">
+        <f>VLOOKUP(A21,popn!$A$2:$B$248,2,0)</f>
+        <v>45593300</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9385280574211485</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>['Ukraine', 1.93852805742115],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1">
-        <v>88383.891280419644</v>
+        <v>88044.0968255185</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>['Ukraine', 88383],</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>['Thailand', 88044],</v>
+      </c>
+      <c r="D22">
+        <f>VLOOKUP(A22,popn!$A$2:$B$248,2,0)</f>
+        <v>66785001</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3183214121014761</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>['Thailand', 1.31832141210148],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1">
-        <v>88044.0968255185</v>
+        <v>84860.632914475194</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>['Thailand', 88044],</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>['Turkey', 84860],</v>
+      </c>
+      <c r="D23">
+        <f>VLOOKUP(A23,popn!$A$2:$B$248,2,0)</f>
+        <v>73997128</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1468098182739632</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>['Turkey', 1.14680981827396],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
-        <v>84860.632914475194</v>
+        <v>83894.730079754285</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>['Turkey', 84860],</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>['Poland', 83894],</v>
+      </c>
+      <c r="D24">
+        <f>VLOOKUP(A24,popn!$A$2:$B$248,2,0)</f>
+        <v>38535873</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1770553914726234</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>['Poland', 2.17705539147262],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1">
-        <v>83894.730079754285</v>
+        <v>79616.824283165581</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>['Poland', 83894],</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>['Kazakhstan', 79616],</v>
+      </c>
+      <c r="D25">
+        <f>VLOOKUP(A25,popn!$A$2:$B$248,2,0)</f>
+        <v>16791425</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>4.7415168327384718</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>['Kazakhstan', 4.74151683273847],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
-        <v>79616.824283165581</v>
+        <v>75676.701894265265</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>['Kazakhstan', 79616],</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>['Spain', 75676],</v>
+      </c>
+      <c r="D26">
+        <f>VLOOKUP(A26,popn!$A$2:$B$248,2,0)</f>
+        <v>46773055</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.617955078928782</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>['Spain', 1.61795507892878],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1">
-        <v>75676.701894265265</v>
+        <v>71558.817520396173</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>['Spain', 75676],</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>['Taiwan', 71558],</v>
+      </c>
+      <c r="D27" t="e">
+        <f>VLOOKUP(A27,popn!$A$2:$B$248,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E27" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B28" s="1">
-        <v>71558.817520396173</v>
+        <v>58952.860837533932</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>['Taiwan', 71558],</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>['Malaysia', 58952],</v>
+      </c>
+      <c r="D28">
+        <f>VLOOKUP(A28,popn!$A$2:$B$248,2,0)</f>
+        <v>29239927</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0161767448165633</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>['Malaysia', 2.01617674481656],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1">
-        <v>58952.860837533932</v>
+        <v>58649.554507574256</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>['Malaysia', 58952],</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>['Egypt', 58649],</v>
+      </c>
+      <c r="D29">
+        <f>VLOOKUP(A29,popn!$A$2:$B$248,2,0)</f>
+        <v>80721874</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.72656334152468083</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>['Egypt', 0.726563341524681],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B30" s="1">
-        <v>58649.554507574256</v>
+        <v>56599.572881389635</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>['Egypt', 58649],</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>['Venezuela', 56599],</v>
+      </c>
+      <c r="D30">
+        <f>VLOOKUP(A30,popn!$A$2:$B$248,2,0)</f>
+        <v>29954782</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8895004103648505</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>['Venezuela', 1.88950041036485],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B31" s="1">
-        <v>56599.572881389635</v>
+        <v>53547.937624577215</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>['Venezuela', 56599],</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>['Argentina', 53547],</v>
+      </c>
+      <c r="D31">
+        <f>VLOOKUP(A31,popn!$A$2:$B$248,2,0)</f>
+        <v>41086927</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3032840743864154</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>['Argentina', 1.30328407438642],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1">
-        <v>53547.937624577215</v>
+        <v>46720.745295175308</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>['Argentina', 53547],</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>['United Arab Emirates', 46720],</v>
+      </c>
+      <c r="D32">
+        <f>VLOOKUP(A32,popn!$A$2:$B$248,2,0)</f>
+        <v>9205651</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0752244784399609</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>['United Arab Emirates', 5.07522447843996],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1">
-        <v>46720.745295175308</v>
+        <v>45421.391169338378</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>['United Arab Emirates', 46720],</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>['Netherlands', 45421],</v>
+      </c>
+      <c r="D33">
+        <f>VLOOKUP(A33,popn!$A$2:$B$248,2,0)</f>
+        <v>16754962</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>2.710921765703699</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>['Netherlands', 2.7109217657037],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1">
-        <v>45421.391169338378</v>
+        <v>44624.503473974044</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>['Netherlands', 45421],</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>['Vietnam', 44624],</v>
+      </c>
+      <c r="D34">
+        <f>VLOOKUP(A34,popn!$A$2:$B$248,2,0)</f>
+        <v>88772900</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.50268160073596824</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="2"/>
+        <v>['Vietnam', 0.502681600735968],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1">
-        <v>44624.503473974044</v>
+        <v>44051.877142625519</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>['Vietnam', 44624],</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>['Pakistan', 44051],</v>
+      </c>
+      <c r="D35">
+        <f>VLOOKUP(A35,popn!$A$2:$B$248,2,0)</f>
+        <v>179160111</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24587993888118054</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="2"/>
+        <v>['Pakistan', 0.245879938881181],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1">
-        <v>44051.877142625519</v>
+        <v>37669.831280628729</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>['Pakistan', 44051],</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>['Algeria', 37669],</v>
+      </c>
+      <c r="D36">
+        <f>VLOOKUP(A36,popn!$A$2:$B$248,2,0)</f>
+        <v>38481705</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>0.97890234542956778</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>['Algeria', 0.978902345429568],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1">
-        <v>37669.831280628729</v>
+        <v>30047.57970204344</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>['Algeria', 37669],</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>['Uzbekistan', 30047],</v>
+      </c>
+      <c r="D37">
+        <f>VLOOKUP(A37,popn!$A$2:$B$248,2,0)</f>
+        <v>29774500</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0091715965689916</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="2"/>
+        <v>['Uzbekistan', 1.00917159656899],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B38" s="1">
-        <v>30047.57970204344</v>
+        <v>28288.208953162346</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>['Uzbekistan', 30047],</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>['Czech Republic', 28288],</v>
+      </c>
+      <c r="D38">
+        <f>VLOOKUP(A38,popn!$A$2:$B$248,2,0)</f>
+        <v>10510785</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6913507367111347</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="2"/>
+        <v>['Czech Republic', 2.69135073671113],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="B39" s="1">
-        <v>28288.208953162346</v>
+        <v>27050.534949886813</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>['Czech Republic', 28288],</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>['Belgium', 27050],</v>
+      </c>
+      <c r="D39">
+        <f>VLOOKUP(A39,popn!$A$2:$B$248,2,0)</f>
+        <v>11128246</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4307995123298687</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="2"/>
+        <v>['Belgium', 2.43079951232987],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B40" s="1">
-        <v>27050.534949886813</v>
+        <v>26357.955150148671</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>['Belgium', 27050],</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>['Kuwait', 26357],</v>
+      </c>
+      <c r="D40">
+        <f>VLOOKUP(A40,popn!$A$2:$B$248,2,0)</f>
+        <v>3250496</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="1"/>
+        <v>8.1089025029252984</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="2"/>
+        <v>['Kuwait', 8.1089025029253],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1">
-        <v>26357.955150148671</v>
+        <v>24778.588030401319</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>['Kuwait', 26357],</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>['Chile', 24778],</v>
+      </c>
+      <c r="D41">
+        <f>VLOOKUP(A41,popn!$A$2:$B$248,2,0)</f>
+        <v>17464814</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4187719394206728</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="2"/>
+        <v>['Chile', 1.41877193942067],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B42" s="1">
-        <v>24778.588030401319</v>
+        <v>24662.641373500301</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>['Chile', 24778],</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>['Qatar', 24662],</v>
+      </c>
+      <c r="D42">
+        <f>VLOOKUP(A42,popn!$A$2:$B$248,2,0)</f>
+        <v>2050514</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>12.027541081650893</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="2"/>
+        <v>['Qatar', 12.0275410816509],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1">
-        <v>24662.641373500301</v>
+        <v>23624.612841412923</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>['Qatar', 24662],</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>['Philippines', 23624],</v>
+      </c>
+      <c r="D43">
+        <f>VLOOKUP(A43,popn!$A$2:$B$248,2,0)</f>
+        <v>96706764</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24429121463947367</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="2"/>
+        <v>['Philippines', 0.244291214639474],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B44" s="1">
-        <v>23624.612841412923</v>
+        <v>22289.532632336344</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>['Philippines', 23624],</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>['Greece', 22289],</v>
+      </c>
+      <c r="D44">
+        <f>VLOOKUP(A44,popn!$A$2:$B$248,2,0)</f>
+        <v>11092771</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0093746307695652</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="2"/>
+        <v>['Greece', 2.00937463076957],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B45" s="1">
-        <v>22289.532632336344</v>
+        <v>22210.831051712248</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>['Greece', 22289],</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>['Romania', 22210],</v>
+      </c>
+      <c r="D45">
+        <f>VLOOKUP(A45,popn!$A$2:$B$248,2,0)</f>
+        <v>20058035</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1073283625096999</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="2"/>
+        <v>['Romania', 1.1073283625097],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B46" s="1">
-        <v>22210.831051712248</v>
+        <v>21981.374513227292</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>['Romania', 22210],</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>['Colombia', 21981],</v>
+      </c>
+      <c r="D46">
+        <f>VLOOKUP(A46,popn!$A$2:$B$248,2,0)</f>
+        <v>47704427</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46078269660858295</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="2"/>
+        <v>['Colombia', 0.460782696608583],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
-        <v>21981.374513227292</v>
+        <v>20928.274947645612</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>['Colombia', 21981],</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>['Israel', 20928],</v>
+      </c>
+      <c r="D47">
+        <f>VLOOKUP(A47,popn!$A$2:$B$248,2,0)</f>
+        <v>7910500</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6456323807149502</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="2"/>
+        <v>['Israel', 2.64563238071495],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B48" s="1">
-        <v>20928.274947645612</v>
+        <v>17805.006345243961</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>['Israel', 20928],</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>['Peru', 17805],</v>
+      </c>
+      <c r="D48">
+        <f>VLOOKUP(A48,popn!$A$2:$B$248,2,0)</f>
+        <v>29987800</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="1"/>
+        <v>0.59374166645248938</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="2"/>
+        <v>['Peru', 0.593741666452489],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1">
-        <v>17805.006345243961</v>
+        <v>17707.259472079972</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>['Peru', 17805],</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>['Bangladesh', 17707],</v>
+      </c>
+      <c r="D49">
+        <f>VLOOKUP(A49,popn!$A$2:$B$248,2,0)</f>
+        <v>154695368</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11446535019768642</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="2"/>
+        <v>['Bangladesh', 0.114465350197686],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="B50" s="1">
-        <v>17707.259472079972</v>
+        <v>16907.219335105743</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>['Bangladesh', 17707],</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>['Belarus', 16907],</v>
+      </c>
+      <c r="D50">
+        <f>VLOOKUP(A50,popn!$A$2:$B$248,2,0)</f>
+        <v>9464000</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7864771064143854</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="2"/>
+        <v>['Belarus', 1.78647710641439],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B51" s="1">
-        <v>16907.219335105743</v>
+        <v>16312.18374570173</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>['Belarus', 16907],</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>['Austria', 16312],</v>
+      </c>
+      <c r="D51">
+        <f>VLOOKUP(A51,popn!$A$2:$B$248,2,0)</f>
+        <v>8429991</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9350179313004876</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="2"/>
+        <v>['Austria', 1.93501793130049],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B52" s="1">
-        <v>16312.18374570173</v>
+        <v>15835.25608083871</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v>['Austria', 16312],</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>['Norway', 15835],</v>
+      </c>
+      <c r="D52">
+        <f>VLOOKUP(A52,popn!$A$2:$B$248,2,0)</f>
+        <v>5018573</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1553304257681831</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="2"/>
+        <v>['Norway', 3.15533042576818],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B53" s="1">
-        <v>15835.25608083871</v>
+        <v>15059.267237126263</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>['Norway', 15835],</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>['Turkmenistan', 15059],</v>
+      </c>
+      <c r="D53">
+        <f>VLOOKUP(A53,popn!$A$2:$B$248,2,0)</f>
+        <v>5172931</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9111672351953395</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="2"/>
+        <v>['Turkmenistan', 2.91116723519534],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B54" s="1">
-        <v>15059.267237126263</v>
+        <v>14367.716966656817</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>['Turkmenistan', 15059],</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>['Portugal', 14367],</v>
+      </c>
+      <c r="D54">
+        <f>VLOOKUP(A54,popn!$A$2:$B$248,2,0)</f>
+        <v>10514844</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3664222661464893</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="2"/>
+        <v>['Portugal', 1.36642226614649],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B55" s="1">
-        <v>14367.716966656817</v>
+        <v>13897.073742635057</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>['Portugal', 14367],</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>['Azerbaijan', 13897],</v>
+      </c>
+      <c r="D55">
+        <f>VLOOKUP(A55,popn!$A$2:$B$248,2,0)</f>
+        <v>9295784</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4949867319028773</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="2"/>
+        <v>['Azerbaijan', 1.49498673190288],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B56" s="1">
-        <v>13897.073742635057</v>
+        <v>13055.362836911692</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>['Azerbaijan', 13897],</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>['Finland', 13055],</v>
+      </c>
+      <c r="D56">
+        <f>VLOOKUP(A56,popn!$A$2:$B$248,2,0)</f>
+        <v>5413971</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4114209028662499</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="2"/>
+        <v>['Finland', 2.41142090286625],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B57" s="1">
-        <v>13055.362836911692</v>
+        <v>12835.629274219658</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>['Finland', 13055],</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>['Trinidad &amp; Tobago', 12835],</v>
+      </c>
+      <c r="D57">
+        <f>VLOOKUP(A57,popn!$A$2:$B$248,2,0)</f>
+        <v>1337439</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="1"/>
+        <v>9.597169870341494</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="2"/>
+        <v>['Trinidad &amp; Tobago', 9.59716987034149],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B58" s="1">
-        <v>12835.629274219658</v>
+        <v>12675.221851083235</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>['Trinidad &amp; Tobago', 12835],</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>['Hungary', 12675],</v>
+      </c>
+      <c r="D58">
+        <f>VLOOKUP(A58,popn!$A$2:$B$248,2,0)</f>
+        <v>9920362</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2776975125588397</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="2"/>
+        <v>['Hungary', 1.27769751255884],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B59" s="1">
-        <v>12675.221851083235</v>
+        <v>12414.359814007172</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v>['Hungary', 12675],</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>['Bulgaria', 12414],</v>
+      </c>
+      <c r="D59">
+        <f>VLOOKUP(A59,popn!$A$2:$B$248,2,0)</f>
+        <v>7305888</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="1"/>
+        <v>1.699226680453789</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="2"/>
+        <v>['Bulgaria', 1.69922668045379],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B60" s="1">
-        <v>12414.359814007172</v>
+        <v>12232.977073612488</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v>['Bulgaria', 12414],</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>['Sweden', 12232],</v>
+      </c>
+      <c r="D60">
+        <f>VLOOKUP(A60,popn!$A$2:$B$248,2,0)</f>
+        <v>9519374</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2850610842280688</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="2"/>
+        <v>['Sweden', 1.28506108422807],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B61" s="1">
-        <v>12232.977073612488</v>
+        <v>10483.038448486963</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v>['Sweden', 12232],</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>['China Hong Kong SAR', 10483],</v>
+      </c>
+      <c r="D61" t="e">
+        <f>VLOOKUP(A61,popn!$A$2:$B$248,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E61" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B62" s="1">
-        <v>10483.038448486963</v>
+        <v>10366.176395978035</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v>['China Hong Kong SAR', 10483],</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>['Switzerland', 10366],</v>
+      </c>
+      <c r="D62">
+        <f>VLOOKUP(A62,popn!$A$2:$B$248,2,0)</f>
+        <v>7996861</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2962806776281386</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="2"/>
+        <v>['Switzerland', 1.29628067762814],</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B63" s="1">
-        <v>10366.176395978035</v>
+        <v>10007.632989994278</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v>['Switzerland', 10366],</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>['Denmark', 10007],</v>
+      </c>
+      <c r="D63">
+        <f>VLOOKUP(A63,popn!$A$2:$B$248,2,0)</f>
+        <v>5591572</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7897709248837854</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="2"/>
+        <v>['Denmark', 1.78977092488379],</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B64" s="1">
-        <v>10007.632989994278</v>
+        <v>9889.6927845552054</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v>['Denmark', 10007],</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>['Republic of Ireland', 9889],</v>
+      </c>
+      <c r="D64">
+        <f>VLOOKUP(A64,popn!$A$2:$B$248,2,0)</f>
+        <v>4586897</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" si="1"/>
+        <v>2.15607474607675</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="2"/>
+        <v>['Republic of Ireland', 2.15607474607675],</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B65" s="1">
-        <v>9889.6927845552054</v>
+        <v>9689.3621084826627</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
-        <v>['Republic of Ireland', 9889],</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>['Slovakia', 9689],</v>
+      </c>
+      <c r="D65" t="e">
+        <f>VLOOKUP(A65,popn!$A$2:$B$248,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E65" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B66" s="1">
-        <v>9689.3621084826627</v>
+        <v>9513.9366238645707</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="0"/>
-        <v>['Slovakia', 9689],</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <f t="shared" ref="C66:C69" si="3">CONCATENATE("['",A66,"', ",INT(B66),"],")</f>
+        <v>['Ecuador', 9513],</v>
+      </c>
+      <c r="D66">
+        <f>VLOOKUP(A66,popn!$A$2:$B$248,2,0)</f>
+        <v>15492264</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" si="1"/>
+        <v>0.6141088625822908</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="2"/>
+        <v>['Ecuador', 0.614108862582291],</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B67" s="1">
-        <v>9513.9366238645707</v>
+        <v>8852.4563185252373</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C70" si="1">CONCATENATE("['",A67,"', ",INT(B67),"],")</f>
-        <v>['Ecuador', 9513],</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <f t="shared" si="3"/>
+        <v>['New Zealand', 8852],</v>
+      </c>
+      <c r="D67">
+        <f>VLOOKUP(A67,popn!$A$2:$B$248,2,0)</f>
+        <v>4408100</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" ref="E67:E69" si="4">B67/D67*1000</f>
+        <v>2.0082249310417728</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F69" si="5">CONCATENATE("['",A67,"', ",E67,"],")</f>
+        <v>['New Zealand', 2.00822493104177],</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="B68" s="1">
-        <v>8852.4563185252373</v>
+        <v>3718.3905708440489</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="1"/>
-        <v>['New Zealand', 8852],</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <f t="shared" si="3"/>
+        <v>['Lithuania', 3718],</v>
+      </c>
+      <c r="D68">
+        <f>VLOOKUP(A68,popn!$A$2:$B$248,2,0)</f>
+        <v>2987773</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2445358368403654</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="5"/>
+        <v>['Lithuania', 1.24453583684037],</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B69" s="1">
-        <v>3718.3905708440489</v>
+        <v>3587.6411665787928</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="1"/>
-        <v>['Lithuania', 3718],</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="1">
-        <v>3587.6411665787928</v>
-      </c>
-      <c r="C70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['Singapore', 3587],</v>
       </c>
+      <c r="D69">
+        <f>VLOOKUP(A69,popn!$A$2:$B$248,2,0)</f>
+        <v>5312400</v>
+      </c>
+      <c r="E69" s="2">
+        <f t="shared" si="4"/>
+        <v>0.67533340233769912</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="5"/>
+        <v>['Singapore', 0.675333402337699],</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C70">
+  <autoFilter ref="A1:C69">
     <sortState ref="A2:C70">
       <sortCondition descending="1" ref="B1:B70"/>
     </sortState>
@@ -11286,4 +12658,2012 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B248"/>
+  <sheetViews>
+    <sheetView topLeftCell="A94" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>102384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3">
+        <v>78360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>29824536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5">
+        <v>20820525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>2900489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7">
+        <v>362466629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>9205651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>41086927</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10">
+        <v>2969081</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11">
+        <v>55128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12">
+        <v>89069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <v>22728300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>8429991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>9295784</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16">
+        <v>9849569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17">
+        <v>11128246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18">
+        <v>10050702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19">
+        <v>16460141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20">
+        <v>154695368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>7305888</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22">
+        <v>1317827</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23">
+        <v>371960</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24">
+        <v>3833916</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>9464000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26">
+        <v>324060</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27">
+        <v>64798</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28">
+        <v>10496285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>198656019</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30">
+        <v>283221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31">
+        <v>412238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32">
+        <v>741822</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33">
+        <v>2003910</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34">
+        <v>4525209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>34752128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36">
+        <v>104408027</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>7996861</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38">
+        <v>161235</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>17464814</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>1350695000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41">
+        <v>19839750</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42">
+        <v>21699631</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43">
+        <v>4337051</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>47704427</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45">
+        <v>717503</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46">
+        <v>494401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47">
+        <v>4805295</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48">
+        <v>6964458</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49">
+        <v>11270957</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50">
+        <v>152086</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51">
+        <v>57570</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52">
+        <v>1128994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>10510785</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54">
+        <v>80425823</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55">
+        <v>859652</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56">
+        <v>71684</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57">
+        <v>5591572</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58">
+        <v>10276621</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59">
+        <v>38481705</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60">
+        <v>1991555125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61">
+        <v>2233703405</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62">
+        <v>270476087</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63">
+        <v>895431689</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64">
+        <v>15492264</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65">
+        <v>80721874</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66">
+        <v>336198768</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67">
+        <v>6130922</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68">
+        <v>46773055</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69">
+        <v>1322696</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70">
+        <v>91728849</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71">
+        <v>505608515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72">
+        <v>436224882</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73">
+        <v>5413971</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74">
+        <v>874742</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75">
+        <v>65649570</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76">
+        <v>49506</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77">
+        <v>103395</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78">
+        <v>1632572</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79">
+        <v>63700300</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>153</v>
+      </c>
+      <c r="B80">
+        <v>4490700</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81">
+        <v>25366462</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82">
+        <v>11451273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>156</v>
+      </c>
+      <c r="B83">
+        <v>1791225</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84">
+        <v>1663558</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85">
+        <v>736296</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86">
+        <v>11092771</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87">
+        <v>105483</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88">
+        <v>56810</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>161</v>
+      </c>
+      <c r="B89">
+        <v>15082831</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90">
+        <v>162810</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>163</v>
+      </c>
+      <c r="B91">
+        <v>795369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92">
+        <v>1299453762</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>165</v>
+      </c>
+      <c r="B93">
+        <v>7154600</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94">
+        <v>7935846</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95">
+        <v>655971763</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96">
+        <v>4267558</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97">
+        <v>10173775</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98">
+        <v>9920362</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99">
+        <v>246864191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>170</v>
+      </c>
+      <c r="B100">
+        <v>85284</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>63</v>
+      </c>
+      <c r="B101">
+        <v>1236686732</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>25</v>
+      </c>
+      <c r="B102">
+        <v>4586897</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103">
+        <v>76424443</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>171</v>
+      </c>
+      <c r="B104">
+        <v>32578209</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>172</v>
+      </c>
+      <c r="B105">
+        <v>320716</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>47</v>
+      </c>
+      <c r="B106">
+        <v>7910500</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107">
+        <v>59539717</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108">
+        <v>2707805</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>174</v>
+      </c>
+      <c r="B109">
+        <v>6318000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>65</v>
+      </c>
+      <c r="B110">
+        <v>127561489</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>27</v>
+      </c>
+      <c r="B111">
+        <v>16791425</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112">
+        <v>43178141</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113">
+        <v>5607200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114">
+        <v>14864646</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115">
+        <v>100786</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>179</v>
+      </c>
+      <c r="B116">
+        <v>53584</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>71</v>
+      </c>
+      <c r="B117">
+        <v>50004441</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>180</v>
+      </c>
+      <c r="B118">
+        <v>1807106</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>48</v>
+      </c>
+      <c r="B119">
+        <v>3250496</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>181</v>
+      </c>
+      <c r="B120">
+        <v>581379260</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>182</v>
+      </c>
+      <c r="B121">
+        <v>6645827</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>183</v>
+      </c>
+      <c r="B122">
+        <v>4424888</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>184</v>
+      </c>
+      <c r="B123">
+        <v>4190435</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>185</v>
+      </c>
+      <c r="B124">
+        <v>6154623</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>186</v>
+      </c>
+      <c r="B125">
+        <v>180870</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>187</v>
+      </c>
+      <c r="B126">
+        <v>608545934</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>188</v>
+      </c>
+      <c r="B127">
+        <v>877943413</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>189</v>
+      </c>
+      <c r="B128">
+        <v>830035274</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>190</v>
+      </c>
+      <c r="B129">
+        <v>36656</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>191</v>
+      </c>
+      <c r="B130">
+        <v>20328000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>192</v>
+      </c>
+      <c r="B131">
+        <v>2523370023</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132">
+        <v>5743727652</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>194</v>
+      </c>
+      <c r="B133">
+        <v>2051545</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>28</v>
+      </c>
+      <c r="B134">
+        <v>2987773</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>195</v>
+      </c>
+      <c r="B135">
+        <v>530946</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>196</v>
+      </c>
+      <c r="B136">
+        <v>2034319</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>197</v>
+      </c>
+      <c r="B137">
+        <v>556783</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>198</v>
+      </c>
+      <c r="B138">
+        <v>30959</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>199</v>
+      </c>
+      <c r="B139">
+        <v>32521143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>200</v>
+      </c>
+      <c r="B140">
+        <v>37579</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>201</v>
+      </c>
+      <c r="B141">
+        <v>3559519</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>202</v>
+      </c>
+      <c r="B142">
+        <v>22293914</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>203</v>
+      </c>
+      <c r="B143">
+        <v>338442</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>204</v>
+      </c>
+      <c r="B144">
+        <v>395316900</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145">
+        <v>120847477</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>205</v>
+      </c>
+      <c r="B146">
+        <v>52555</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>206</v>
+      </c>
+      <c r="B147">
+        <v>4913692378</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>207</v>
+      </c>
+      <c r="B148">
+        <v>2105575</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>208</v>
+      </c>
+      <c r="B149">
+        <v>14853572</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>209</v>
+      </c>
+      <c r="B150">
+        <v>419455</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>210</v>
+      </c>
+      <c r="B151">
+        <v>52797319</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>211</v>
+      </c>
+      <c r="B152">
+        <v>339560601</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>212</v>
+      </c>
+      <c r="B153">
+        <v>621081</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>213</v>
+      </c>
+      <c r="B154">
+        <v>2796484</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>214</v>
+      </c>
+      <c r="B155">
+        <v>53305</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>215</v>
+      </c>
+      <c r="B156">
+        <v>25203395</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>216</v>
+      </c>
+      <c r="B157">
+        <v>3796141</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>217</v>
+      </c>
+      <c r="B158">
+        <v>1255882</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>218</v>
+      </c>
+      <c r="B159">
+        <v>15906483</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>66</v>
+      </c>
+      <c r="B160">
+        <v>29239927</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>219</v>
+      </c>
+      <c r="B161">
+        <v>348690611</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>220</v>
+      </c>
+      <c r="B162">
+        <v>2259393</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>221</v>
+      </c>
+      <c r="B163">
+        <v>258000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>222</v>
+      </c>
+      <c r="B164">
+        <v>17157042</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>223</v>
+      </c>
+      <c r="B165">
+        <v>168833776</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>224</v>
+      </c>
+      <c r="B166">
+        <v>5991733</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>29</v>
+      </c>
+      <c r="B167">
+        <v>16754962</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>225</v>
+      </c>
+      <c r="B168">
+        <v>249928024</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>30</v>
+      </c>
+      <c r="B169">
+        <v>5018573</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>226</v>
+      </c>
+      <c r="B170">
+        <v>27474377</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>67</v>
+      </c>
+      <c r="B171">
+        <v>4408100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>227</v>
+      </c>
+      <c r="B172">
+        <v>1049525738</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>228</v>
+      </c>
+      <c r="B173">
+        <v>1254290705</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>229</v>
+      </c>
+      <c r="B174">
+        <v>3314001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>230</v>
+      </c>
+      <c r="B175">
+        <v>19823626</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>68</v>
+      </c>
+      <c r="B176">
+        <v>179160111</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>231</v>
+      </c>
+      <c r="B177">
+        <v>3802281</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>9</v>
+      </c>
+      <c r="B178">
+        <v>29987800</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>69</v>
+      </c>
+      <c r="B179">
+        <v>96706764</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>232</v>
+      </c>
+      <c r="B180">
+        <v>20754</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>233</v>
+      </c>
+      <c r="B181">
+        <v>7167010</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>31</v>
+      </c>
+      <c r="B182">
+        <v>38535873</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>234</v>
+      </c>
+      <c r="B183">
+        <v>3651545</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>283</v>
+      </c>
+      <c r="B184">
+        <v>24763188</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>32</v>
+      </c>
+      <c r="B185">
+        <v>10514844</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>235</v>
+      </c>
+      <c r="B186">
+        <v>6687361</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>236</v>
+      </c>
+      <c r="B187">
+        <v>2252782</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>237</v>
+      </c>
+      <c r="B188">
+        <v>273814</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>49</v>
+      </c>
+      <c r="B189">
+        <v>2050514</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>33</v>
+      </c>
+      <c r="B190">
+        <v>20058035</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>34</v>
+      </c>
+      <c r="B191">
+        <v>143178000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>238</v>
+      </c>
+      <c r="B192">
+        <v>11457801</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>239</v>
+      </c>
+      <c r="B193">
+        <v>1649249388</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>50</v>
+      </c>
+      <c r="B194">
+        <v>28287855</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>240</v>
+      </c>
+      <c r="B195">
+        <v>37195349</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>241</v>
+      </c>
+      <c r="B196">
+        <v>13726021</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>70</v>
+      </c>
+      <c r="B197">
+        <v>5312400</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>242</v>
+      </c>
+      <c r="B198">
+        <v>549598</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>243</v>
+      </c>
+      <c r="B199">
+        <v>5978727</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>244</v>
+      </c>
+      <c r="B200">
+        <v>6297394</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>245</v>
+      </c>
+      <c r="B201">
+        <v>31247</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>246</v>
+      </c>
+      <c r="B202">
+        <v>10195134</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>247</v>
+      </c>
+      <c r="B203">
+        <v>7199077</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>248</v>
+      </c>
+      <c r="B204">
+        <v>911507191</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>249</v>
+      </c>
+      <c r="B205">
+        <v>10837527</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>250</v>
+      </c>
+      <c r="B206">
+        <v>912243487</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>251</v>
+      </c>
+      <c r="B207">
+        <v>29040866</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>252</v>
+      </c>
+      <c r="B208">
+        <v>188098</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>253</v>
+      </c>
+      <c r="B209">
+        <v>534541</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>254</v>
+      </c>
+      <c r="B210">
+        <v>5407579</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>255</v>
+      </c>
+      <c r="B211">
+        <v>2057159</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>37</v>
+      </c>
+      <c r="B212">
+        <v>9519374</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>256</v>
+      </c>
+      <c r="B213">
+        <v>1230985</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>257</v>
+      </c>
+      <c r="B214">
+        <v>39088</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>258</v>
+      </c>
+      <c r="B215">
+        <v>88303</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>259</v>
+      </c>
+      <c r="B216">
+        <v>22399254</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>260</v>
+      </c>
+      <c r="B217">
+        <v>32427</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>261</v>
+      </c>
+      <c r="B218">
+        <v>12448175</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>262</v>
+      </c>
+      <c r="B219">
+        <v>6642928</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>73</v>
+      </c>
+      <c r="B220">
+        <v>66785001</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>263</v>
+      </c>
+      <c r="B221">
+        <v>8008990</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>40</v>
+      </c>
+      <c r="B222">
+        <v>5172931</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>264</v>
+      </c>
+      <c r="B223">
+        <v>1148958</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>265</v>
+      </c>
+      <c r="B224">
+        <v>104941</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>10</v>
+      </c>
+      <c r="B225">
+        <v>1337439</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>266</v>
+      </c>
+      <c r="B226">
+        <v>10777500</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>39</v>
+      </c>
+      <c r="B227">
+        <v>73997128</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>267</v>
+      </c>
+      <c r="B228">
+        <v>9860</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>268</v>
+      </c>
+      <c r="B229">
+        <v>47783107</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>269</v>
+      </c>
+      <c r="B230">
+        <v>36345860</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>41</v>
+      </c>
+      <c r="B231">
+        <v>45593300</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>270</v>
+      </c>
+      <c r="B232">
+        <v>2390322355</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>271</v>
+      </c>
+      <c r="B233">
+        <v>3395253</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>0</v>
+      </c>
+      <c r="B234">
+        <v>313873685</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>43</v>
+      </c>
+      <c r="B235">
+        <v>29774500</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>272</v>
+      </c>
+      <c r="B236">
+        <v>109373</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>11</v>
+      </c>
+      <c r="B237">
+        <v>29954782</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>273</v>
+      </c>
+      <c r="B238">
+        <v>105275</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>74</v>
+      </c>
+      <c r="B239">
+        <v>88772900</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>274</v>
+      </c>
+      <c r="B240">
+        <v>247262</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>275</v>
+      </c>
+      <c r="B241">
+        <v>4046901</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>276</v>
+      </c>
+      <c r="B242">
+        <v>7043181414</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>277</v>
+      </c>
+      <c r="B243">
+        <v>188889</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>278</v>
+      </c>
+      <c r="B244">
+        <v>23852409</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>56</v>
+      </c>
+      <c r="B245">
+        <v>52341695</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>279</v>
+      </c>
+      <c r="B246">
+        <v>65705093</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>280</v>
+      </c>
+      <c r="B247">
+        <v>14075099</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>281</v>
+      </c>
+      <c r="B248">
+        <v>13724317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new graphic contents
</commit_message>
<xml_diff>
--- a/3-climate-change/data/CO2_emissions_2012.xlsx
+++ b/3-climate-change/data/CO2_emissions_2012.xlsx
@@ -13,7 +13,7 @@
     <sheet name="popn" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CURATED!$A$1:$C$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CURATED!$A$1:$F$69</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -944,10 +944,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -990,7 +994,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1010,6 +1014,8 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1028,6 +1034,8 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -10998,8 +11006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11060,7 +11068,7 @@
         <v>1396790.7648451091</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C65" si="0">CONCATENATE("['",A3,"', ",INT(B3),"],")</f>
+        <f>CONCATENATE("['",A3,"', ",INT(B3),"],")</f>
         <v>['US', 1396790],</v>
       </c>
       <c r="D3">
@@ -11068,11 +11076,11 @@
         <v>313873685</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E66" si="1">B3/D3*1000</f>
+        <f>B3/D3*1000</f>
         <v>4.4501684327091935</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="2">CONCATENATE("['",A3,"', ",E3,"],")</f>
+        <f>CONCATENATE("['",A3,"', ",E3,"],")</f>
         <v>['US', 4.45016843270919],</v>
       </c>
     </row>
@@ -11084,7 +11092,7 @@
         <v>611226.32316958916</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A4,"', ",INT(B4),"],")</f>
         <v>['India', 611226],</v>
       </c>
       <c r="D4">
@@ -11092,11 +11100,11 @@
         <v>1236686732</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="1"/>
+        <f>B4/D4*1000</f>
         <v>0.49424507221897584</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A4,"', ",E4,"],")</f>
         <v>['India', 0.494245072218976],</v>
       </c>
     </row>
@@ -11108,7 +11116,7 @@
         <v>491840.33543909399</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A5,"', ",INT(B5),"],")</f>
         <v>['Russian Federation', 491840],</v>
       </c>
       <c r="D5">
@@ -11116,11 +11124,11 @@
         <v>143178000</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f>B5/D5*1000</f>
         <v>3.4351669630745922</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A5,"', ",E5,"],")</f>
         <v>['Russian Federation', 3.43516696307459],</v>
       </c>
     </row>
@@ -11132,7 +11140,7 @@
         <v>342270.02191037923</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A6,"', ",INT(B6),"],")</f>
         <v>['Japan', 342270],</v>
       </c>
       <c r="D6">
@@ -11140,11 +11148,11 @@
         <v>127561489</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f>B6/D6*1000</f>
         <v>2.6831767533724791</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A6,"', ",E6,"],")</f>
         <v>['Japan', 2.68317675337248],</v>
       </c>
     </row>
@@ -11156,7 +11164,7 @@
         <v>199716.14896148487</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A7,"', ",INT(B7),"],")</f>
         <v>['Germany', 199716],</v>
       </c>
       <c r="D7">
@@ -11164,11 +11172,11 @@
         <v>80425823</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f>B7/D7*1000</f>
         <v>2.4832341344083586</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A7,"', ",E7,"],")</f>
         <v>['Germany', 2.48323413440836],</v>
       </c>
     </row>
@@ -11180,7 +11188,7 @@
         <v>166679.15746470925</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A8,"', ",INT(B8),"],")</f>
         <v>['South Korea', 166679],</v>
       </c>
       <c r="D8">
@@ -11188,11 +11196,11 @@
         <v>50004441</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f>B8/D8*1000</f>
         <v>3.3332870867351412</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A8,"', ",E8,"],")</f>
         <v>['South Korea', 3.33328708673514],</v>
       </c>
     </row>
@@ -11204,7 +11212,7 @@
         <v>164497.67410158212</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A9,"', ",INT(B9),"],")</f>
         <v>['Iran', 164497],</v>
       </c>
       <c r="D9">
@@ -11212,11 +11220,11 @@
         <v>76424443</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f>B9/D9*1000</f>
         <v>2.1524222832946536</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A9,"', ",E9,"],")</f>
         <v>['Iran', 2.15242228329465],</v>
       </c>
     </row>
@@ -11228,7 +11236,7 @@
         <v>137877.70810957171</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A10,"', ",INT(B10),"],")</f>
         <v>['Saudi Arabia', 137877],</v>
       </c>
       <c r="D10">
@@ -11236,11 +11244,11 @@
         <v>28287855</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f>B10/D10*1000</f>
         <v>4.8740955477031296</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A10,"', ",E10,"],")</f>
         <v>['Saudi Arabia', 4.87409554770313],</v>
       </c>
     </row>
@@ -11252,7 +11260,7 @@
         <v>137819.83011260908</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A11,"', ",INT(B11),"],")</f>
         <v>['Canada', 137819],</v>
       </c>
       <c r="D11">
@@ -11260,11 +11268,11 @@
         <v>34752128</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f>B11/D11*1000</f>
         <v>3.9657954215813507</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A11,"', ",E11,"],")</f>
         <v>['Canada', 3.96579542158135],</v>
       </c>
     </row>
@@ -11276,7 +11284,7 @@
         <v>129987.63422779723</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A12,"', ",INT(B12),"],")</f>
         <v>['Indonesia', 129987],</v>
       </c>
       <c r="D12">
@@ -11284,11 +11292,11 @@
         <v>246864191</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f>B12/D12*1000</f>
         <v>0.52655524359868466</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A12,"', ",E12,"],")</f>
         <v>['Indonesia', 0.526555243598685],</v>
       </c>
     </row>
@@ -11300,7 +11308,7 @@
         <v>129942.37582630581</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A13,"', ",INT(B13),"],")</f>
         <v>['Mexico', 129942],</v>
       </c>
       <c r="D13">
@@ -11308,11 +11316,11 @@
         <v>120847477</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f>B13/D13*1000</f>
         <v>1.0752593190365556</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A13,"', ",E13,"],")</f>
         <v>['Mexico', 1.07525931903656],</v>
       </c>
     </row>
@@ -11324,7 +11332,7 @@
         <v>128494.04064963351</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A14,"', ",INT(B14),"],")</f>
         <v>['United Kingdom', 128494],</v>
       </c>
       <c r="D14">
@@ -11332,11 +11340,11 @@
         <v>63700300</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f>B14/D14*1000</f>
         <v>2.0171653924649258</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A14,"', ",E14,"],")</f>
         <v>['United Kingdom', 2.01716539246493],</v>
       </c>
     </row>
@@ -11348,7 +11356,7 @@
         <v>125741.87230816028</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A15,"', ",INT(B15),"],")</f>
         <v>['South Africa', 125741],</v>
       </c>
       <c r="D15">
@@ -11356,11 +11364,11 @@
         <v>52341695</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f>B15/D15*1000</f>
         <v>2.4023270990394998</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A15,"', ",E15,"],")</f>
         <v>['South Africa', 2.4023270990395],</v>
       </c>
     </row>
@@ -11372,7 +11380,7 @@
         <v>122082.41549725691</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A16,"', ",INT(B16),"],")</f>
         <v>['Brazil', 122082],</v>
       </c>
       <c r="D16">
@@ -11380,11 +11388,11 @@
         <v>198656019</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f>B16/D16*1000</f>
         <v>0.614541739594897</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A16,"', ",E16,"],")</f>
         <v>['Brazil', 0.614541739594897],</v>
       </c>
     </row>
@@ -11396,7 +11404,7 @@
         <v>108880.73748252774</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A17,"', ",INT(B17),"],")</f>
         <v>['Other Africa', 108880],</v>
       </c>
       <c r="D17" t="e">
@@ -11404,7 +11412,7 @@
         <v>#N/A</v>
       </c>
       <c r="E17" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f>B17/D17*1000</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -11416,7 +11424,7 @@
         <v>102368.62639672708</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A18,"', ",INT(B18),"],")</f>
         <v>['Italy', 102368],</v>
       </c>
       <c r="D18">
@@ -11424,11 +11432,11 @@
         <v>59539717</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f>B18/D18*1000</f>
         <v>1.7193334391684643</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A18,"', ",E18,"],")</f>
         <v>['Italy', 1.71933343916846],</v>
       </c>
     </row>
@@ -11440,7 +11448,7 @@
         <v>101147.00533811742</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A19,"', ",INT(B19),"],")</f>
         <v>['Australia', 101147],</v>
       </c>
       <c r="D19">
@@ -11448,11 +11456,11 @@
         <v>22728300</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="1"/>
+        <f>B19/D19*1000</f>
         <v>4.4502670828050244</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A19,"', ",E19,"],")</f>
         <v>['Australia', 4.45026708280502],</v>
       </c>
     </row>
@@ -11464,7 +11472,7 @@
         <v>93712.565440615203</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A20,"', ",INT(B20),"],")</f>
         <v>['France', 93712],</v>
       </c>
       <c r="D20">
@@ -11472,11 +11480,11 @@
         <v>65649570</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="1"/>
+        <f>B20/D20*1000</f>
         <v>1.4274665537126168</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A20,"', ",E20,"],")</f>
         <v>['France', 1.42746655371262],</v>
       </c>
     </row>
@@ -11488,7 +11496,7 @@
         <v>88383.891280419644</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A21,"', ",INT(B21),"],")</f>
         <v>['Ukraine', 88383],</v>
       </c>
       <c r="D21">
@@ -11496,11 +11504,11 @@
         <v>45593300</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="1"/>
+        <f>B21/D21*1000</f>
         <v>1.9385280574211485</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A21,"', ",E21,"],")</f>
         <v>['Ukraine', 1.93852805742115],</v>
       </c>
     </row>
@@ -11512,7 +11520,7 @@
         <v>88044.0968255185</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A22,"', ",INT(B22),"],")</f>
         <v>['Thailand', 88044],</v>
       </c>
       <c r="D22">
@@ -11520,11 +11528,11 @@
         <v>66785001</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="1"/>
+        <f>B22/D22*1000</f>
         <v>1.3183214121014761</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A22,"', ",E22,"],")</f>
         <v>['Thailand', 1.31832141210148],</v>
       </c>
     </row>
@@ -11536,7 +11544,7 @@
         <v>84860.632914475194</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A23,"', ",INT(B23),"],")</f>
         <v>['Turkey', 84860],</v>
       </c>
       <c r="D23">
@@ -11544,11 +11552,11 @@
         <v>73997128</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="1"/>
+        <f>B23/D23*1000</f>
         <v>1.1468098182739632</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A23,"', ",E23,"],")</f>
         <v>['Turkey', 1.14680981827396],</v>
       </c>
     </row>
@@ -11560,7 +11568,7 @@
         <v>83894.730079754285</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A24,"', ",INT(B24),"],")</f>
         <v>['Poland', 83894],</v>
       </c>
       <c r="D24">
@@ -11568,11 +11576,11 @@
         <v>38535873</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="1"/>
+        <f>B24/D24*1000</f>
         <v>2.1770553914726234</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A24,"', ",E24,"],")</f>
         <v>['Poland', 2.17705539147262],</v>
       </c>
     </row>
@@ -11584,7 +11592,7 @@
         <v>79616.824283165581</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A25,"', ",INT(B25),"],")</f>
         <v>['Kazakhstan', 79616],</v>
       </c>
       <c r="D25">
@@ -11592,11 +11600,11 @@
         <v>16791425</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="1"/>
+        <f>B25/D25*1000</f>
         <v>4.7415168327384718</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A25,"', ",E25,"],")</f>
         <v>['Kazakhstan', 4.74151683273847],</v>
       </c>
     </row>
@@ -11608,7 +11616,7 @@
         <v>75676.701894265265</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A26,"', ",INT(B26),"],")</f>
         <v>['Spain', 75676],</v>
       </c>
       <c r="D26">
@@ -11616,11 +11624,11 @@
         <v>46773055</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="1"/>
+        <f>B26/D26*1000</f>
         <v>1.617955078928782</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A26,"', ",E26,"],")</f>
         <v>['Spain', 1.61795507892878],</v>
       </c>
     </row>
@@ -11632,7 +11640,7 @@
         <v>71558.817520396173</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A27,"', ",INT(B27),"],")</f>
         <v>['Taiwan', 71558],</v>
       </c>
       <c r="D27" t="e">
@@ -11640,7 +11648,7 @@
         <v>#N/A</v>
       </c>
       <c r="E27" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f>B27/D27*1000</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -11652,7 +11660,7 @@
         <v>58952.860837533932</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A28,"', ",INT(B28),"],")</f>
         <v>['Malaysia', 58952],</v>
       </c>
       <c r="D28">
@@ -11660,11 +11668,11 @@
         <v>29239927</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="1"/>
+        <f>B28/D28*1000</f>
         <v>2.0161767448165633</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A28,"', ",E28,"],")</f>
         <v>['Malaysia', 2.01617674481656],</v>
       </c>
     </row>
@@ -11676,7 +11684,7 @@
         <v>58649.554507574256</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A29,"', ",INT(B29),"],")</f>
         <v>['Egypt', 58649],</v>
       </c>
       <c r="D29">
@@ -11684,11 +11692,11 @@
         <v>80721874</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="1"/>
+        <f>B29/D29*1000</f>
         <v>0.72656334152468083</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A29,"', ",E29,"],")</f>
         <v>['Egypt', 0.726563341524681],</v>
       </c>
     </row>
@@ -11700,7 +11708,7 @@
         <v>56599.572881389635</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A30,"', ",INT(B30),"],")</f>
         <v>['Venezuela', 56599],</v>
       </c>
       <c r="D30">
@@ -11708,11 +11716,11 @@
         <v>29954782</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="1"/>
+        <f>B30/D30*1000</f>
         <v>1.8895004103648505</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A30,"', ",E30,"],")</f>
         <v>['Venezuela', 1.88950041036485],</v>
       </c>
     </row>
@@ -11724,7 +11732,7 @@
         <v>53547.937624577215</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A31,"', ",INT(B31),"],")</f>
         <v>['Argentina', 53547],</v>
       </c>
       <c r="D31">
@@ -11732,11 +11740,11 @@
         <v>41086927</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="1"/>
+        <f>B31/D31*1000</f>
         <v>1.3032840743864154</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A31,"', ",E31,"],")</f>
         <v>['Argentina', 1.30328407438642],</v>
       </c>
     </row>
@@ -11748,7 +11756,7 @@
         <v>46720.745295175308</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A32,"', ",INT(B32),"],")</f>
         <v>['United Arab Emirates', 46720],</v>
       </c>
       <c r="D32">
@@ -11756,11 +11764,11 @@
         <v>9205651</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="1"/>
+        <f>B32/D32*1000</f>
         <v>5.0752244784399609</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A32,"', ",E32,"],")</f>
         <v>['United Arab Emirates', 5.07522447843996],</v>
       </c>
     </row>
@@ -11772,7 +11780,7 @@
         <v>45421.391169338378</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A33,"', ",INT(B33),"],")</f>
         <v>['Netherlands', 45421],</v>
       </c>
       <c r="D33">
@@ -11780,11 +11788,11 @@
         <v>16754962</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="1"/>
+        <f>B33/D33*1000</f>
         <v>2.710921765703699</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A33,"', ",E33,"],")</f>
         <v>['Netherlands', 2.7109217657037],</v>
       </c>
     </row>
@@ -11796,7 +11804,7 @@
         <v>44624.503473974044</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A34,"', ",INT(B34),"],")</f>
         <v>['Vietnam', 44624],</v>
       </c>
       <c r="D34">
@@ -11804,11 +11812,11 @@
         <v>88772900</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="1"/>
+        <f>B34/D34*1000</f>
         <v>0.50268160073596824</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A34,"', ",E34,"],")</f>
         <v>['Vietnam', 0.502681600735968],</v>
       </c>
     </row>
@@ -11820,7 +11828,7 @@
         <v>44051.877142625519</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A35,"', ",INT(B35),"],")</f>
         <v>['Pakistan', 44051],</v>
       </c>
       <c r="D35">
@@ -11828,11 +11836,11 @@
         <v>179160111</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="1"/>
+        <f>B35/D35*1000</f>
         <v>0.24587993888118054</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A35,"', ",E35,"],")</f>
         <v>['Pakistan', 0.245879938881181],</v>
       </c>
     </row>
@@ -11844,7 +11852,7 @@
         <v>37669.831280628729</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A36,"', ",INT(B36),"],")</f>
         <v>['Algeria', 37669],</v>
       </c>
       <c r="D36">
@@ -11852,11 +11860,11 @@
         <v>38481705</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="1"/>
+        <f>B36/D36*1000</f>
         <v>0.97890234542956778</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A36,"', ",E36,"],")</f>
         <v>['Algeria', 0.978902345429568],</v>
       </c>
     </row>
@@ -11868,7 +11876,7 @@
         <v>30047.57970204344</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A37,"', ",INT(B37),"],")</f>
         <v>['Uzbekistan', 30047],</v>
       </c>
       <c r="D37">
@@ -11876,11 +11884,11 @@
         <v>29774500</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="1"/>
+        <f>B37/D37*1000</f>
         <v>1.0091715965689916</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A37,"', ",E37,"],")</f>
         <v>['Uzbekistan', 1.00917159656899],</v>
       </c>
     </row>
@@ -11892,7 +11900,7 @@
         <v>28288.208953162346</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A38,"', ",INT(B38),"],")</f>
         <v>['Czech Republic', 28288],</v>
       </c>
       <c r="D38">
@@ -11900,11 +11908,11 @@
         <v>10510785</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="1"/>
+        <f>B38/D38*1000</f>
         <v>2.6913507367111347</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A38,"', ",E38,"],")</f>
         <v>['Czech Republic', 2.69135073671113],</v>
       </c>
     </row>
@@ -11916,7 +11924,7 @@
         <v>27050.534949886813</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A39,"', ",INT(B39),"],")</f>
         <v>['Belgium', 27050],</v>
       </c>
       <c r="D39">
@@ -11924,11 +11932,11 @@
         <v>11128246</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="1"/>
+        <f>B39/D39*1000</f>
         <v>2.4307995123298687</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A39,"', ",E39,"],")</f>
         <v>['Belgium', 2.43079951232987],</v>
       </c>
     </row>
@@ -11940,7 +11948,7 @@
         <v>26357.955150148671</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A40,"', ",INT(B40),"],")</f>
         <v>['Kuwait', 26357],</v>
       </c>
       <c r="D40">
@@ -11948,11 +11956,11 @@
         <v>3250496</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="1"/>
+        <f>B40/D40*1000</f>
         <v>8.1089025029252984</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A40,"', ",E40,"],")</f>
         <v>['Kuwait', 8.1089025029253],</v>
       </c>
     </row>
@@ -11964,7 +11972,7 @@
         <v>24778.588030401319</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A41,"', ",INT(B41),"],")</f>
         <v>['Chile', 24778],</v>
       </c>
       <c r="D41">
@@ -11972,11 +11980,11 @@
         <v>17464814</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="1"/>
+        <f>B41/D41*1000</f>
         <v>1.4187719394206728</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A41,"', ",E41,"],")</f>
         <v>['Chile', 1.41877193942067],</v>
       </c>
     </row>
@@ -11988,7 +11996,7 @@
         <v>24662.641373500301</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A42,"', ",INT(B42),"],")</f>
         <v>['Qatar', 24662],</v>
       </c>
       <c r="D42">
@@ -11996,11 +12004,11 @@
         <v>2050514</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="1"/>
+        <f>B42/D42*1000</f>
         <v>12.027541081650893</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A42,"', ",E42,"],")</f>
         <v>['Qatar', 12.0275410816509],</v>
       </c>
     </row>
@@ -12012,7 +12020,7 @@
         <v>23624.612841412923</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A43,"', ",INT(B43),"],")</f>
         <v>['Philippines', 23624],</v>
       </c>
       <c r="D43">
@@ -12020,11 +12028,11 @@
         <v>96706764</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="1"/>
+        <f>B43/D43*1000</f>
         <v>0.24429121463947367</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A43,"', ",E43,"],")</f>
         <v>['Philippines', 0.244291214639474],</v>
       </c>
     </row>
@@ -12036,7 +12044,7 @@
         <v>22289.532632336344</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A44,"', ",INT(B44),"],")</f>
         <v>['Greece', 22289],</v>
       </c>
       <c r="D44">
@@ -12044,11 +12052,11 @@
         <v>11092771</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="1"/>
+        <f>B44/D44*1000</f>
         <v>2.0093746307695652</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A44,"', ",E44,"],")</f>
         <v>['Greece', 2.00937463076957],</v>
       </c>
     </row>
@@ -12060,7 +12068,7 @@
         <v>22210.831051712248</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A45,"', ",INT(B45),"],")</f>
         <v>['Romania', 22210],</v>
       </c>
       <c r="D45">
@@ -12068,11 +12076,11 @@
         <v>20058035</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="1"/>
+        <f>B45/D45*1000</f>
         <v>1.1073283625096999</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A45,"', ",E45,"],")</f>
         <v>['Romania', 1.1073283625097],</v>
       </c>
     </row>
@@ -12084,7 +12092,7 @@
         <v>21981.374513227292</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A46,"', ",INT(B46),"],")</f>
         <v>['Colombia', 21981],</v>
       </c>
       <c r="D46">
@@ -12092,11 +12100,11 @@
         <v>47704427</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="1"/>
+        <f>B46/D46*1000</f>
         <v>0.46078269660858295</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A46,"', ",E46,"],")</f>
         <v>['Colombia', 0.460782696608583],</v>
       </c>
     </row>
@@ -12108,7 +12116,7 @@
         <v>20928.274947645612</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A47,"', ",INT(B47),"],")</f>
         <v>['Israel', 20928],</v>
       </c>
       <c r="D47">
@@ -12116,11 +12124,11 @@
         <v>7910500</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="1"/>
+        <f>B47/D47*1000</f>
         <v>2.6456323807149502</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A47,"', ",E47,"],")</f>
         <v>['Israel', 2.64563238071495],</v>
       </c>
     </row>
@@ -12132,7 +12140,7 @@
         <v>17805.006345243961</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A48,"', ",INT(B48),"],")</f>
         <v>['Peru', 17805],</v>
       </c>
       <c r="D48">
@@ -12140,11 +12148,11 @@
         <v>29987800</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="1"/>
+        <f>B48/D48*1000</f>
         <v>0.59374166645248938</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A48,"', ",E48,"],")</f>
         <v>['Peru', 0.593741666452489],</v>
       </c>
     </row>
@@ -12156,7 +12164,7 @@
         <v>17707.259472079972</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A49,"', ",INT(B49),"],")</f>
         <v>['Bangladesh', 17707],</v>
       </c>
       <c r="D49">
@@ -12164,11 +12172,11 @@
         <v>154695368</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="1"/>
+        <f>B49/D49*1000</f>
         <v>0.11446535019768642</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A49,"', ",E49,"],")</f>
         <v>['Bangladesh', 0.114465350197686],</v>
       </c>
     </row>
@@ -12180,7 +12188,7 @@
         <v>16907.219335105743</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A50,"', ",INT(B50),"],")</f>
         <v>['Belarus', 16907],</v>
       </c>
       <c r="D50">
@@ -12188,11 +12196,11 @@
         <v>9464000</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="1"/>
+        <f>B50/D50*1000</f>
         <v>1.7864771064143854</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A50,"', ",E50,"],")</f>
         <v>['Belarus', 1.78647710641439],</v>
       </c>
     </row>
@@ -12204,7 +12212,7 @@
         <v>16312.18374570173</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A51,"', ",INT(B51),"],")</f>
         <v>['Austria', 16312],</v>
       </c>
       <c r="D51">
@@ -12212,11 +12220,11 @@
         <v>8429991</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="1"/>
+        <f>B51/D51*1000</f>
         <v>1.9350179313004876</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A51,"', ",E51,"],")</f>
         <v>['Austria', 1.93501793130049],</v>
       </c>
     </row>
@@ -12228,7 +12236,7 @@
         <v>15835.25608083871</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A52,"', ",INT(B52),"],")</f>
         <v>['Norway', 15835],</v>
       </c>
       <c r="D52">
@@ -12236,11 +12244,11 @@
         <v>5018573</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="1"/>
+        <f>B52/D52*1000</f>
         <v>3.1553304257681831</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A52,"', ",E52,"],")</f>
         <v>['Norway', 3.15533042576818],</v>
       </c>
     </row>
@@ -12252,7 +12260,7 @@
         <v>15059.267237126263</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A53,"', ",INT(B53),"],")</f>
         <v>['Turkmenistan', 15059],</v>
       </c>
       <c r="D53">
@@ -12260,11 +12268,11 @@
         <v>5172931</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="1"/>
+        <f>B53/D53*1000</f>
         <v>2.9111672351953395</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A53,"', ",E53,"],")</f>
         <v>['Turkmenistan', 2.91116723519534],</v>
       </c>
     </row>
@@ -12276,7 +12284,7 @@
         <v>14367.716966656817</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A54,"', ",INT(B54),"],")</f>
         <v>['Portugal', 14367],</v>
       </c>
       <c r="D54">
@@ -12284,11 +12292,11 @@
         <v>10514844</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="1"/>
+        <f>B54/D54*1000</f>
         <v>1.3664222661464893</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A54,"', ",E54,"],")</f>
         <v>['Portugal', 1.36642226614649],</v>
       </c>
     </row>
@@ -12300,7 +12308,7 @@
         <v>13897.073742635057</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A55,"', ",INT(B55),"],")</f>
         <v>['Azerbaijan', 13897],</v>
       </c>
       <c r="D55">
@@ -12308,11 +12316,11 @@
         <v>9295784</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="1"/>
+        <f>B55/D55*1000</f>
         <v>1.4949867319028773</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A55,"', ",E55,"],")</f>
         <v>['Azerbaijan', 1.49498673190288],</v>
       </c>
     </row>
@@ -12324,7 +12332,7 @@
         <v>13055.362836911692</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A56,"', ",INT(B56),"],")</f>
         <v>['Finland', 13055],</v>
       </c>
       <c r="D56">
@@ -12332,11 +12340,11 @@
         <v>5413971</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="1"/>
+        <f>B56/D56*1000</f>
         <v>2.4114209028662499</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A56,"', ",E56,"],")</f>
         <v>['Finland', 2.41142090286625],</v>
       </c>
     </row>
@@ -12348,7 +12356,7 @@
         <v>12835.629274219658</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A57,"', ",INT(B57),"],")</f>
         <v>['Trinidad &amp; Tobago', 12835],</v>
       </c>
       <c r="D57">
@@ -12356,11 +12364,11 @@
         <v>1337439</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="1"/>
+        <f>B57/D57*1000</f>
         <v>9.597169870341494</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A57,"', ",E57,"],")</f>
         <v>['Trinidad &amp; Tobago', 9.59716987034149],</v>
       </c>
     </row>
@@ -12372,7 +12380,7 @@
         <v>12675.221851083235</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A58,"', ",INT(B58),"],")</f>
         <v>['Hungary', 12675],</v>
       </c>
       <c r="D58">
@@ -12380,11 +12388,11 @@
         <v>9920362</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="1"/>
+        <f>B58/D58*1000</f>
         <v>1.2776975125588397</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A58,"', ",E58,"],")</f>
         <v>['Hungary', 1.27769751255884],</v>
       </c>
     </row>
@@ -12396,7 +12404,7 @@
         <v>12414.359814007172</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A59,"', ",INT(B59),"],")</f>
         <v>['Bulgaria', 12414],</v>
       </c>
       <c r="D59">
@@ -12404,11 +12412,11 @@
         <v>7305888</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="1"/>
+        <f>B59/D59*1000</f>
         <v>1.699226680453789</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A59,"', ",E59,"],")</f>
         <v>['Bulgaria', 1.69922668045379],</v>
       </c>
     </row>
@@ -12420,7 +12428,7 @@
         <v>12232.977073612488</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A60,"', ",INT(B60),"],")</f>
         <v>['Sweden', 12232],</v>
       </c>
       <c r="D60">
@@ -12428,11 +12436,11 @@
         <v>9519374</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="1"/>
+        <f>B60/D60*1000</f>
         <v>1.2850610842280688</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A60,"', ",E60,"],")</f>
         <v>['Sweden', 1.28506108422807],</v>
       </c>
     </row>
@@ -12444,7 +12452,7 @@
         <v>10483.038448486963</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A61,"', ",INT(B61),"],")</f>
         <v>['China Hong Kong SAR', 10483],</v>
       </c>
       <c r="D61" t="e">
@@ -12452,7 +12460,7 @@
         <v>#N/A</v>
       </c>
       <c r="E61" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f>B61/D61*1000</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -12464,7 +12472,7 @@
         <v>10366.176395978035</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A62,"', ",INT(B62),"],")</f>
         <v>['Switzerland', 10366],</v>
       </c>
       <c r="D62">
@@ -12472,11 +12480,11 @@
         <v>7996861</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="1"/>
+        <f>B62/D62*1000</f>
         <v>1.2962806776281386</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A62,"', ",E62,"],")</f>
         <v>['Switzerland', 1.29628067762814],</v>
       </c>
     </row>
@@ -12488,7 +12496,7 @@
         <v>10007.632989994278</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A63,"', ",INT(B63),"],")</f>
         <v>['Denmark', 10007],</v>
       </c>
       <c r="D63">
@@ -12496,11 +12504,11 @@
         <v>5591572</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="1"/>
+        <f>B63/D63*1000</f>
         <v>1.7897709248837854</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A63,"', ",E63,"],")</f>
         <v>['Denmark', 1.78977092488379],</v>
       </c>
     </row>
@@ -12512,7 +12520,7 @@
         <v>9889.6927845552054</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A64,"', ",INT(B64),"],")</f>
         <v>['Republic of Ireland', 9889],</v>
       </c>
       <c r="D64">
@@ -12520,11 +12528,11 @@
         <v>4586897</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="1"/>
+        <f>B64/D64*1000</f>
         <v>2.15607474607675</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A64,"', ",E64,"],")</f>
         <v>['Republic of Ireland', 2.15607474607675],</v>
       </c>
     </row>
@@ -12536,7 +12544,7 @@
         <v>9689.3621084826627</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("['",A65,"', ",INT(B65),"],")</f>
         <v>['Slovakia', 9689],</v>
       </c>
       <c r="D65" t="e">
@@ -12544,7 +12552,7 @@
         <v>#N/A</v>
       </c>
       <c r="E65" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f>B65/D65*1000</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -12556,7 +12564,7 @@
         <v>9513.9366238645707</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C69" si="3">CONCATENATE("['",A66,"', ",INT(B66),"],")</f>
+        <f>CONCATENATE("['",A66,"', ",INT(B66),"],")</f>
         <v>['Ecuador', 9513],</v>
       </c>
       <c r="D66">
@@ -12564,11 +12572,11 @@
         <v>15492264</v>
       </c>
       <c r="E66" s="2">
-        <f t="shared" si="1"/>
+        <f>B66/D66*1000</f>
         <v>0.6141088625822908</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("['",A66,"', ",E66,"],")</f>
         <v>['Ecuador', 0.614108862582291],</v>
       </c>
     </row>
@@ -12580,7 +12588,7 @@
         <v>8852.4563185252373</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE("['",A67,"', ",INT(B67),"],")</f>
         <v>['New Zealand', 8852],</v>
       </c>
       <c r="D67">
@@ -12588,11 +12596,11 @@
         <v>4408100</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E69" si="4">B67/D67*1000</f>
+        <f>B67/D67*1000</f>
         <v>2.0082249310417728</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F69" si="5">CONCATENATE("['",A67,"', ",E67,"],")</f>
+        <f>CONCATENATE("['",A67,"', ",E67,"],")</f>
         <v>['New Zealand', 2.00822493104177],</v>
       </c>
     </row>
@@ -12604,7 +12612,7 @@
         <v>3718.3905708440489</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE("['",A68,"', ",INT(B68),"],")</f>
         <v>['Lithuania', 3718],</v>
       </c>
       <c r="D68">
@@ -12612,11 +12620,11 @@
         <v>2987773</v>
       </c>
       <c r="E68" s="2">
-        <f t="shared" si="4"/>
+        <f>B68/D68*1000</f>
         <v>1.2445358368403654</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="5"/>
+        <f>CONCATENATE("['",A68,"', ",E68,"],")</f>
         <v>['Lithuania', 1.24453583684037],</v>
       </c>
     </row>
@@ -12628,7 +12636,7 @@
         <v>3587.6411665787928</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE("['",A69,"', ",INT(B69),"],")</f>
         <v>['Singapore', 3587],</v>
       </c>
       <c r="D69">
@@ -12636,20 +12644,16 @@
         <v>5312400</v>
       </c>
       <c r="E69" s="2">
-        <f t="shared" si="4"/>
+        <f>B69/D69*1000</f>
         <v>0.67533340233769912</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="5"/>
+        <f>CONCATENATE("['",A69,"', ",E69,"],")</f>
         <v>['Singapore', 0.675333402337699],</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C69">
-    <sortState ref="A2:C70">
-      <sortCondition descending="1" ref="B1:B70"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:F69"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>